<commit_message>
feat: Añadir asserts a tests de SOAT
</commit_message>
<xml_diff>
--- a/data/segmentacion_soat.xlsx
+++ b/data/segmentacion_soat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/plantilla_seguimiento/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F07EAF-F68B-2440-8726-CFF94EFBD039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A68FDDF-CDDF-C447-B173-4C5B24F5FE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="3" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="2" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
   </bookViews>
   <sheets>
     <sheet name="add_spe_Sucursales" sheetId="9" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10052" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10103" uniqueCount="206">
   <si>
     <t>Amparo_Desc</t>
   </si>
@@ -587,6 +587,117 @@
   </si>
   <si>
     <t>tipo_ajuste</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>711</t>
+  </si>
+  <si>
+    <t>712</t>
+  </si>
+  <si>
+    <t>721</t>
+  </si>
+  <si>
+    <t>722</t>
+  </si>
+  <si>
+    <t>731</t>
+  </si>
+  <si>
+    <t>732</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>910</t>
+  </si>
+  <si>
+    <t>920</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>211</t>
+  </si>
+  <si>
+    <t>212</t>
+  </si>
+  <si>
+    <t>221</t>
+  </si>
+  <si>
+    <t>222</t>
+  </si>
+  <si>
+    <t>231</t>
+  </si>
+  <si>
+    <t>232</t>
+  </si>
+  <si>
+    <t>310</t>
+  </si>
+  <si>
+    <t>320</t>
+  </si>
+  <si>
+    <t>330</t>
+  </si>
+  <si>
+    <t>410</t>
+  </si>
+  <si>
+    <t>420</t>
+  </si>
+  <si>
+    <t>430</t>
+  </si>
+  <si>
+    <t>511</t>
+  </si>
+  <si>
+    <t>512</t>
+  </si>
+  <si>
+    <t>521</t>
+  </si>
+  <si>
+    <t>522</t>
+  </si>
+  <si>
+    <t>531</t>
+  </si>
+  <si>
+    <t>532</t>
+  </si>
+  <si>
+    <t>611</t>
+  </si>
+  <si>
+    <t>612</t>
+  </si>
+  <si>
+    <t>621</t>
+  </si>
+  <si>
+    <t>622</t>
   </si>
 </sst>
 </file>
@@ -1814,8 +1925,8 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1840,8 +1951,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="15">
-        <v>100</v>
+      <c r="A2" s="15" t="s">
+        <v>169</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>126</v>
@@ -1855,8 +1966,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="15">
-        <v>110</v>
+      <c r="A3" s="15" t="s">
+        <v>170</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>126</v>
@@ -1870,8 +1981,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="15">
-        <v>120</v>
+      <c r="A4" s="15" t="s">
+        <v>171</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>126</v>
@@ -1885,8 +1996,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="15">
-        <v>140</v>
+      <c r="A5" s="15" t="s">
+        <v>172</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>126</v>
@@ -1900,8 +2011,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="15">
-        <v>150</v>
+      <c r="A6" s="15" t="s">
+        <v>173</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>126</v>
@@ -1915,8 +2026,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="15">
-        <v>711</v>
+      <c r="A7" s="15" t="s">
+        <v>174</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>126</v>
@@ -1930,8 +2041,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="15">
-        <v>712</v>
+      <c r="A8" s="15" t="s">
+        <v>175</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>126</v>
@@ -1945,8 +2056,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="15">
-        <v>721</v>
+      <c r="A9" s="15" t="s">
+        <v>176</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>126</v>
@@ -1960,8 +2071,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="15">
-        <v>722</v>
+      <c r="A10" s="15" t="s">
+        <v>177</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>126</v>
@@ -1975,8 +2086,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="15">
-        <v>731</v>
+      <c r="A11" s="15" t="s">
+        <v>178</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>126</v>
@@ -1990,8 +2101,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="15">
-        <v>732</v>
+      <c r="A12" s="15" t="s">
+        <v>179</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>126</v>
@@ -2005,8 +2116,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="15">
-        <v>810</v>
+      <c r="A13" s="15" t="s">
+        <v>180</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>126</v>
@@ -2020,8 +2131,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="15">
-        <v>910</v>
+      <c r="A14" s="15" t="s">
+        <v>181</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>126</v>
@@ -2035,8 +2146,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="15">
-        <v>920</v>
+      <c r="A15" s="15" t="s">
+        <v>182</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>126</v>
@@ -2050,8 +2161,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>100</v>
+      <c r="A16" t="s">
+        <v>169</v>
       </c>
       <c r="B16" t="s">
         <v>127</v>
@@ -2065,8 +2176,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>110</v>
+      <c r="A17" t="s">
+        <v>170</v>
       </c>
       <c r="B17" t="s">
         <v>127</v>
@@ -2080,8 +2191,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>120</v>
+      <c r="A18" t="s">
+        <v>171</v>
       </c>
       <c r="B18" t="s">
         <v>127</v>
@@ -2095,8 +2206,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>130</v>
+      <c r="A19" t="s">
+        <v>183</v>
       </c>
       <c r="B19" t="s">
         <v>127</v>
@@ -2110,8 +2221,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>140</v>
+      <c r="A20" t="s">
+        <v>172</v>
       </c>
       <c r="B20" t="s">
         <v>127</v>
@@ -2125,8 +2236,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>150</v>
+      <c r="A21" t="s">
+        <v>173</v>
       </c>
       <c r="B21" t="s">
         <v>127</v>
@@ -2140,8 +2251,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>211</v>
+      <c r="A22" t="s">
+        <v>184</v>
       </c>
       <c r="B22" t="s">
         <v>127</v>
@@ -2155,8 +2266,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>212</v>
+      <c r="A23" t="s">
+        <v>185</v>
       </c>
       <c r="B23" t="s">
         <v>127</v>
@@ -2170,8 +2281,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>221</v>
+      <c r="A24" t="s">
+        <v>186</v>
       </c>
       <c r="B24" t="s">
         <v>127</v>
@@ -2185,8 +2296,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>222</v>
+      <c r="A25" t="s">
+        <v>187</v>
       </c>
       <c r="B25" t="s">
         <v>127</v>
@@ -2200,8 +2311,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>231</v>
+      <c r="A26" t="s">
+        <v>188</v>
       </c>
       <c r="B26" t="s">
         <v>127</v>
@@ -2215,8 +2326,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>232</v>
+      <c r="A27" t="s">
+        <v>189</v>
       </c>
       <c r="B27" t="s">
         <v>127</v>
@@ -2230,8 +2341,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>310</v>
+      <c r="A28" t="s">
+        <v>190</v>
       </c>
       <c r="B28" t="s">
         <v>127</v>
@@ -2245,8 +2356,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>320</v>
+      <c r="A29" t="s">
+        <v>191</v>
       </c>
       <c r="B29" t="s">
         <v>127</v>
@@ -2260,8 +2371,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>330</v>
+      <c r="A30" t="s">
+        <v>192</v>
       </c>
       <c r="B30" t="s">
         <v>127</v>
@@ -2275,8 +2386,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>410</v>
+      <c r="A31" t="s">
+        <v>193</v>
       </c>
       <c r="B31" t="s">
         <v>127</v>
@@ -2290,8 +2401,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>420</v>
+      <c r="A32" t="s">
+        <v>194</v>
       </c>
       <c r="B32" t="s">
         <v>127</v>
@@ -2305,8 +2416,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>430</v>
+      <c r="A33" t="s">
+        <v>195</v>
       </c>
       <c r="B33" t="s">
         <v>127</v>
@@ -2320,8 +2431,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>511</v>
+      <c r="A34" t="s">
+        <v>196</v>
       </c>
       <c r="B34" t="s">
         <v>127</v>
@@ -2335,8 +2446,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>512</v>
+      <c r="A35" t="s">
+        <v>197</v>
       </c>
       <c r="B35" t="s">
         <v>127</v>
@@ -2350,8 +2461,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>521</v>
+      <c r="A36" t="s">
+        <v>198</v>
       </c>
       <c r="B36" t="s">
         <v>127</v>
@@ -2365,8 +2476,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>522</v>
+      <c r="A37" t="s">
+        <v>199</v>
       </c>
       <c r="B37" t="s">
         <v>127</v>
@@ -2380,8 +2491,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>531</v>
+      <c r="A38" t="s">
+        <v>200</v>
       </c>
       <c r="B38" t="s">
         <v>127</v>
@@ -2395,8 +2506,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>532</v>
+      <c r="A39" t="s">
+        <v>201</v>
       </c>
       <c r="B39" t="s">
         <v>127</v>
@@ -2410,8 +2521,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>611</v>
+      <c r="A40" t="s">
+        <v>202</v>
       </c>
       <c r="B40" t="s">
         <v>127</v>
@@ -2425,8 +2536,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>612</v>
+      <c r="A41" t="s">
+        <v>203</v>
       </c>
       <c r="B41" t="s">
         <v>127</v>
@@ -2440,8 +2551,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>621</v>
+      <c r="A42" t="s">
+        <v>204</v>
       </c>
       <c r="B42" t="s">
         <v>127</v>
@@ -2455,8 +2566,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>622</v>
+      <c r="A43" t="s">
+        <v>205</v>
       </c>
       <c r="B43" t="s">
         <v>127</v>
@@ -2470,8 +2581,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>711</v>
+      <c r="A44" t="s">
+        <v>174</v>
       </c>
       <c r="B44" t="s">
         <v>127</v>
@@ -2485,8 +2596,8 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>712</v>
+      <c r="A45" t="s">
+        <v>175</v>
       </c>
       <c r="B45" t="s">
         <v>127</v>
@@ -2500,8 +2611,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>721</v>
+      <c r="A46" t="s">
+        <v>176</v>
       </c>
       <c r="B46" t="s">
         <v>127</v>
@@ -2515,8 +2626,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>722</v>
+      <c r="A47" t="s">
+        <v>177</v>
       </c>
       <c r="B47" t="s">
         <v>127</v>
@@ -2530,8 +2641,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>731</v>
+      <c r="A48" t="s">
+        <v>178</v>
       </c>
       <c r="B48" t="s">
         <v>127</v>
@@ -2545,8 +2656,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>732</v>
+      <c r="A49" t="s">
+        <v>179</v>
       </c>
       <c r="B49" t="s">
         <v>127</v>
@@ -2560,8 +2671,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>810</v>
+      <c r="A50" t="s">
+        <v>180</v>
       </c>
       <c r="B50" t="s">
         <v>127</v>
@@ -2575,8 +2686,8 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>910</v>
+      <c r="A51" t="s">
+        <v>181</v>
       </c>
       <c r="B51" t="s">
         <v>127</v>
@@ -2590,8 +2701,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>920</v>
+      <c r="A52" t="s">
+        <v>182</v>
       </c>
       <c r="B52" t="s">
         <v>127</v>
@@ -2617,7 +2728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{923386D2-4D6E-604A-B132-ECEA16641628}">
   <dimension ref="A1:T1207"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -72707,13 +72818,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<Application xmlns="http://www.sap.com/cof/excel/application">
-  <Version>2</Version>
-  <Revision>2.3.1.59180</Revision>
-</Application>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003CF4D88A847C084DB84844F39084E439" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="451e82d02e108cc447a9cc14d7f86033">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="92acd330-8342-45fc-be4b-65850f6282f9" xmlns:ns3="e625656c-bba3-4077-8eff-14104607af5a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2eae878ca301ee5618ce7adadc34258d" ns2:_="" ns3:_="">
     <xsd:import namespace="92acd330-8342-45fc-be4b-65850f6282f9"/>
@@ -72914,7 +73018,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<Application xmlns="http://www.sap.com/cof/excel/application">
+  <Version>2</Version>
+  <Revision>2.3.1.59180</Revision>
+</Application>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="e625656c-bba3-4077-8eff-14104607af5a" xsi:nil="true"/>
@@ -72925,24 +73045,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62D4AD73-2F3B-41AE-8958-0F3FAF115B0E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -72961,7 +73064,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -72979,12 +73098,4 @@
     <ds:schemaRef ds:uri="92acd330-8342-45fc-be4b-65850f6282f9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat: Hacer que la tabla de aperturas y periodicidades se defina desde el Excel de segmentacion
</commit_message>
<xml_diff>
--- a/data/segmentacion_soat.xlsx
+++ b/data/segmentacion_soat.xlsx
@@ -1,29 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/plantilla_seguimiento/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/app-analisis-siniestralidad/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A68FDDF-CDDF-C447-B173-4C5B24F5FE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A25B66-2270-F347-A1C2-04EF1B8D37F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="2" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
+    <workbookView xWindow="30260" yWindow="600" windowWidth="38380" windowHeight="21000" activeTab="2" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
   </bookViews>
   <sheets>
-    <sheet name="add_spe_Sucursales" sheetId="9" r:id="rId1"/>
-    <sheet name="add_spe_Amparos" sheetId="1" r:id="rId2"/>
-    <sheet name="add_spe_Clases" sheetId="10" r:id="rId3"/>
-    <sheet name="Ajustes_Fraude" sheetId="12" r:id="rId4"/>
-    <sheet name="Amparos_Negocio_083" sheetId="4" state="hidden" r:id="rId5"/>
+    <sheet name="Aperturas_Siniestros" sheetId="13" r:id="rId1"/>
+    <sheet name="Aperturas_Primas" sheetId="14" r:id="rId2"/>
+    <sheet name="Aperturas_Expuestos" sheetId="15" r:id="rId3"/>
+    <sheet name="add_spe_Sucursales" sheetId="9" r:id="rId4"/>
+    <sheet name="add_spe_Amparos" sheetId="1" r:id="rId5"/>
+    <sheet name="add_spe_Clases" sheetId="10" r:id="rId6"/>
+    <sheet name="Ajustes_Fraude" sheetId="12" r:id="rId7"/>
+    <sheet name="Amparos_Negocio_083" sheetId="4" state="hidden" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">add_spe_Amparos!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">add_spe_Sucursales!$A$1:$D$28</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Ajustes_Fraude!$D$1:$T$1175</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Amparos_Negocio_083!$A$1:$B$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">add_spe_Amparos!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">add_spe_Sucursales!$A$1:$D$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Ajustes_Fraude!$D$1:$T$1175</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Amparos_Negocio_083!$A$1:$B$80</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -80,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10103" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10296" uniqueCount="208">
   <si>
     <t>Amparo_Desc</t>
   </si>
@@ -699,6 +702,12 @@
   <si>
     <t>622</t>
   </si>
+  <si>
+    <t>Trimestral</t>
+  </si>
+  <si>
+    <t>periodicidad_ocurrencia</t>
+  </si>
 </sst>
 </file>
 
@@ -1282,11 +1291,782 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41685B22-5F49-AB48-8DB6-85DC25F1B5E6}">
+  <sheetPr codeName="Hoja5"/>
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>+B2&amp;"_"&amp;C2&amp;"_"&amp;D2&amp;"_"&amp;E2&amp;"_"&amp;F2</f>
+        <v>01_041_ASESORES_Total_AUTO</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>+B3&amp;"_"&amp;C3&amp;"_"&amp;D3&amp;"_"&amp;E3&amp;"_"&amp;F3</f>
+        <v>01_041_ASESORES_Total_MOTO</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f>+B4&amp;"_"&amp;C4&amp;"_"&amp;D4&amp;"_"&amp;E4&amp;"_"&amp;F4</f>
+        <v>01_041_CERRADO_Total_MOTO</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f>+B5&amp;"_"&amp;C5&amp;"_"&amp;D5&amp;"_"&amp;E5&amp;"_"&amp;F5</f>
+        <v>01_041_CORBETA_Total_AUTO</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="str">
+        <f>+B6&amp;"_"&amp;C6&amp;"_"&amp;D6&amp;"_"&amp;E6&amp;"_"&amp;F6</f>
+        <v>01_041_CORBETA_Total_MOTO</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="str">
+        <f>+B7&amp;"_"&amp;C7&amp;"_"&amp;D7&amp;"_"&amp;E7&amp;"_"&amp;F7</f>
+        <v>01_041_DIGITAL_Total_AUTO</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="str">
+        <f>+B8&amp;"_"&amp;C8&amp;"_"&amp;D8&amp;"_"&amp;E8&amp;"_"&amp;F8</f>
+        <v>01_041_DIGITAL_Total_MOTO</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G8" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="str">
+        <f>+B9&amp;"_"&amp;C9&amp;"_"&amp;D9&amp;"_"&amp;E9&amp;"_"&amp;F9</f>
+        <v>01_041_EXITO_Total_AUTO</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" t="s">
+        <v>120</v>
+      </c>
+      <c r="E9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="str">
+        <f>+B10&amp;"_"&amp;C10&amp;"_"&amp;D10&amp;"_"&amp;E10&amp;"_"&amp;F10</f>
+        <v>01_041_EXITO_Total_MOTO</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G10" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="str">
+        <f>+B11&amp;"_"&amp;C11&amp;"_"&amp;D11&amp;"_"&amp;E11&amp;"_"&amp;F11</f>
+        <v>01_041_RESTO_Total_AUTO</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="str">
+        <f>+B12&amp;"_"&amp;C12&amp;"_"&amp;D12&amp;"_"&amp;E12&amp;"_"&amp;F12</f>
+        <v>01_041_RESTO_Total_MOTO</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" t="s">
+        <v>128</v>
+      </c>
+      <c r="G12" t="s">
+        <v>206</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G12" xr:uid="{22BE6280-917F-9E46-82F3-4F72A7A28E95}">
+      <formula1>"Mensual,Trimestral,Semestral,Anual"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BAF0991-2698-BC44-8533-D730AF03BB1B}">
+  <sheetPr codeName="Hoja6"/>
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9908EB-6C2B-7640-BCA5-4F158164632C}">
+  <sheetPr codeName="Hoja7"/>
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6EE77F-9491-46BE-87E7-0E2AB2968C8E}">
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="132" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
@@ -1772,7 +2552,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A5BF66-2E00-8740-8200-DD18588C6A6C}">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:D8"/>
@@ -1920,13 +2700,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{123C0C09-E83A-4BC0-BA11-233DE6D57A3F}">
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2724,8 +3504,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{923386D2-4D6E-604A-B132-ECEA16641628}">
+  <sheetPr codeName="Hoja8"/>
   <dimension ref="A1:T1207"/>
   <sheetViews>
     <sheetView zoomScaleNormal="70" workbookViewId="0">
@@ -72151,7 +72932,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B135DB0-AD3F-4044-B1FF-A0D4EB51BA31}">
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:E80"/>
@@ -73019,10 +73800,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<Application xmlns="http://www.sap.com/cof/excel/application">
-  <Version>2</Version>
-  <Revision>2.3.1.59180</Revision>
-</Application>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e625656c-bba3-4077-8eff-14104607af5a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="92acd330-8342-45fc-be4b-65850f6282f9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -73035,14 +73820,10 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e625656c-bba3-4077-8eff-14104607af5a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="92acd330-8342-45fc-be4b-65850f6282f9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<Application xmlns="http://www.sap.com/cof/excel/application">
+  <Version>2</Version>
+  <Revision>2.3.1.59180</Revision>
+</Application>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -73065,22 +73846,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -73098,4 +73863,20 @@
     <ds:schemaRef ds:uri="92acd330-8342-45fc-be4b-65850f6282f9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat: Agregar hoja para definir meses a cuadrar contablemente
</commit_message>
<xml_diff>
--- a/data/segmentacion_soat.xlsx
+++ b/data/segmentacion_soat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/app-analisis-siniestralidad/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D50A7C5-3305-DE43-BB4F-EA191A3D6DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167B44B2-B508-CD4D-B147-5BE447F8D0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30260" yWindow="600" windowWidth="38380" windowHeight="21000" activeTab="8" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" firstSheet="2" activeTab="9" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Aperturas_Siniestros" sheetId="13" r:id="rId1"/>
@@ -22,13 +22,15 @@
     <sheet name="Ajustes_Fraude" sheetId="12" r:id="rId7"/>
     <sheet name="Cuadre_Siniestros" sheetId="16" r:id="rId8"/>
     <sheet name="Cuadre_Primas" sheetId="17" r:id="rId9"/>
-    <sheet name="Amparos_Negocio_083" sheetId="4" state="hidden" r:id="rId10"/>
+    <sheet name="Meses_cuadre_siniestros" sheetId="18" r:id="rId10"/>
+    <sheet name="Meses_cuadre_primas" sheetId="19" r:id="rId11"/>
+    <sheet name="Amparos_Negocio_083" sheetId="4" state="hidden" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">add_spe_Amparos!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">add_spe_Sucursales!$A$1:$D$28</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Ajustes_Fraude!$D$1:$T$1175</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Amparos_Negocio_083!$A$1:$B$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Amparos_Negocio_083!$A$1:$B$80</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -85,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10318" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10320" uniqueCount="208">
   <si>
     <t>Amparo_Desc</t>
   </si>
@@ -1294,7 +1296,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41685B22-5F49-AB48-8DB6-85DC25F1B5E6}">
-  <sheetPr codeName="Hoja5"/>
+  <sheetPr codeName="Hoja5">
+    <tabColor theme="4" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1610,6 +1614,4030 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D171BBD-F094-6342-82E9-180B604D24D1}">
+  <sheetPr>
+    <tabColor theme="3" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:A401"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="18">
+        <v>40179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="18">
+        <v>40210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="18">
+        <v>40238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="18">
+        <v>40269</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="18">
+        <v>40299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="18">
+        <v>40330</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="18">
+        <v>40360</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="18">
+        <v>40391</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="18">
+        <v>40422</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="18">
+        <v>40452</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="18">
+        <v>40483</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="18">
+        <v>40513</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="18">
+        <v>40544</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="18">
+        <v>40575</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="18">
+        <v>40603</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="18">
+        <v>40634</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="18">
+        <v>40664</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="18">
+        <v>40695</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="18">
+        <v>40725</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="18">
+        <v>40756</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="18">
+        <v>40787</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="18">
+        <v>40817</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="18">
+        <v>40848</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="18">
+        <v>40878</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="18">
+        <v>40909</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="18">
+        <v>40940</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="18">
+        <v>40969</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="18">
+        <v>41000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="18">
+        <v>41030</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="18">
+        <v>41061</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="18">
+        <v>41091</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="18">
+        <v>41122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="18">
+        <v>41153</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="18">
+        <v>41183</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="18">
+        <v>41214</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="18">
+        <v>41244</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="18">
+        <v>41275</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="18">
+        <v>41306</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="18">
+        <v>41334</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="18">
+        <v>41365</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="18">
+        <v>41395</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="18">
+        <v>41426</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="18">
+        <v>41456</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="18">
+        <v>41487</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="18">
+        <v>41518</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="18">
+        <v>41548</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="18">
+        <v>41579</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="18">
+        <v>41609</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="18">
+        <v>41640</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="18">
+        <v>41671</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="18">
+        <v>41699</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="18">
+        <v>41730</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="18">
+        <v>41760</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="18">
+        <v>41791</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="18">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="18">
+        <v>41852</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="18">
+        <v>41883</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="18">
+        <v>41913</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="18">
+        <v>41944</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="18">
+        <v>41974</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="18">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="18">
+        <v>42036</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="18">
+        <v>42064</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="18">
+        <v>42095</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="18">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="18">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="18">
+        <v>42186</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="18">
+        <v>42217</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="18">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="18">
+        <v>42278</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="18">
+        <v>42309</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="18">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="18">
+        <v>42370</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="18">
+        <v>42401</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" s="18">
+        <v>42430</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="18">
+        <v>42461</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="18">
+        <v>42491</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="18">
+        <v>42522</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" s="18">
+        <v>42552</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="18">
+        <v>42583</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="18">
+        <v>42614</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="18">
+        <v>42644</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" s="18">
+        <v>42675</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="18">
+        <v>42705</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" s="18">
+        <v>42736</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" s="18">
+        <v>42767</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" s="18">
+        <v>42795</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="18">
+        <v>42826</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" s="18">
+        <v>42856</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" s="18">
+        <v>42887</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" s="18">
+        <v>42917</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" s="18">
+        <v>42948</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" s="18">
+        <v>42979</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" s="18">
+        <v>43009</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" s="18">
+        <v>43040</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" s="18">
+        <v>43070</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" s="18">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="18">
+        <v>43132</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" s="18">
+        <v>43160</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" s="18">
+        <v>43191</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" s="18">
+        <v>43221</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" s="18">
+        <v>43252</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" s="18">
+        <v>43282</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" s="18">
+        <v>43313</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" s="18">
+        <v>43344</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" s="18">
+        <v>43374</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" s="18">
+        <v>43405</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" s="18">
+        <v>43435</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" s="18">
+        <v>43466</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" s="18">
+        <v>43497</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" s="18">
+        <v>43525</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" s="18">
+        <v>43556</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" s="18">
+        <v>43586</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" s="18">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" s="18">
+        <v>43647</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" s="18">
+        <v>43678</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" s="18">
+        <v>43709</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" s="18">
+        <v>43739</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" s="18">
+        <v>43770</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" s="18">
+        <v>43800</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" s="18">
+        <v>43831</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123" s="18">
+        <v>43862</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124" s="18">
+        <v>43891</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125" s="18">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126" s="18">
+        <v>43952</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127" s="18">
+        <v>43983</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128" s="18">
+        <v>44013</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129" s="18">
+        <v>44044</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" s="18">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" s="18">
+        <v>44105</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" s="18">
+        <v>44136</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" s="18">
+        <v>44166</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" s="18">
+        <v>44197</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" s="18">
+        <v>44228</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" s="18">
+        <v>44256</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" s="18">
+        <v>44287</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" s="18">
+        <v>44317</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" s="18">
+        <v>44348</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" s="18">
+        <v>44378</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" s="18">
+        <v>44409</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142" s="18">
+        <v>44440</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" s="18">
+        <v>44470</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144" s="18">
+        <v>44501</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145" s="18">
+        <v>44531</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146" s="18">
+        <v>44562</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147" s="18">
+        <v>44593</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148" s="18">
+        <v>44621</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149" s="18">
+        <v>44652</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150" s="18">
+        <v>44682</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151" s="18">
+        <v>44713</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152" s="18">
+        <v>44743</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153" s="18">
+        <v>44774</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154" s="18">
+        <v>44805</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155" s="18">
+        <v>44835</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156" s="18">
+        <v>44866</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" s="18">
+        <v>44896</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158" s="18">
+        <v>44927</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159" s="18">
+        <v>44958</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160" s="18">
+        <v>44986</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" s="18">
+        <v>45017</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" s="18">
+        <v>45047</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" s="18">
+        <v>45078</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" s="18">
+        <v>45108</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165" s="18">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" s="18">
+        <v>45170</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167" s="18">
+        <v>45200</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168" s="18">
+        <v>45231</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169" s="18">
+        <v>45261</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170" s="18">
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171" s="18">
+        <v>45323</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172" s="18">
+        <v>45352</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173" s="18">
+        <v>45383</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174" s="18">
+        <v>45413</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175" s="18">
+        <v>45444</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176" s="18">
+        <v>45474</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177" s="18">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" s="18">
+        <v>45536</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179" s="18">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180" s="18">
+        <v>45597</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181" s="18">
+        <v>45627</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182" s="18">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183" s="18">
+        <v>45689</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184" s="18">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185" s="18">
+        <v>45748</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186" s="18">
+        <v>45778</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187" s="18">
+        <v>45809</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188" s="18">
+        <v>45839</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189" s="18">
+        <v>45870</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190" s="18">
+        <v>45901</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191" s="18">
+        <v>45931</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192" s="18">
+        <v>45962</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193" s="18">
+        <v>45992</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A194" s="18">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195" s="18">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A196" s="18">
+        <v>46082</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A197" s="18">
+        <v>46113</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A198" s="18">
+        <v>46143</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A199" s="18">
+        <v>46174</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A200" s="18">
+        <v>46204</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201" s="18">
+        <v>46235</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A202" s="18">
+        <v>46266</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203" s="18">
+        <v>46296</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A204" s="18">
+        <v>46327</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A205" s="18">
+        <v>46357</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A206" s="18">
+        <v>46388</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A207" s="18">
+        <v>46419</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A208" s="18">
+        <v>46447</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209" s="18">
+        <v>46478</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210" s="18">
+        <v>46508</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A211" s="18">
+        <v>46539</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A212" s="18">
+        <v>46569</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213" s="18">
+        <v>46600</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A214" s="18">
+        <v>46631</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A215" s="18">
+        <v>46661</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A216" s="18">
+        <v>46692</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A217" s="18">
+        <v>46722</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A218" s="18">
+        <v>46753</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A219" s="18">
+        <v>46784</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A220" s="18">
+        <v>46813</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A221" s="18">
+        <v>46844</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A222" s="18">
+        <v>46874</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A223" s="18">
+        <v>46905</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A224" s="18">
+        <v>46935</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A225" s="18">
+        <v>46966</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A226" s="18">
+        <v>46997</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A227" s="18">
+        <v>47027</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A228" s="18">
+        <v>47058</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A229" s="18">
+        <v>47088</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A230" s="18">
+        <v>47119</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A231" s="18">
+        <v>47150</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A232" s="18">
+        <v>47178</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A233" s="18">
+        <v>47209</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A234" s="18">
+        <v>47239</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A235" s="18">
+        <v>47270</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A236" s="18">
+        <v>47300</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A237" s="18">
+        <v>47331</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A238" s="18">
+        <v>47362</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A239" s="18">
+        <v>47392</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A240" s="18">
+        <v>47423</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A241" s="18">
+        <v>47453</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A242" s="18">
+        <v>47484</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A243" s="18">
+        <v>47515</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A244" s="18">
+        <v>47543</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A245" s="18">
+        <v>47574</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A246" s="18">
+        <v>47604</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A247" s="18">
+        <v>47635</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A248" s="18">
+        <v>47665</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A249" s="18">
+        <v>47696</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A250" s="18">
+        <v>47727</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A251" s="18">
+        <v>47757</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A252" s="18">
+        <v>47788</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A253" s="18">
+        <v>47818</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A254" s="18">
+        <v>47849</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A255" s="18">
+        <v>47880</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A256" s="18">
+        <v>47908</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A257" s="18">
+        <v>47939</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A258" s="18">
+        <v>47969</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A259" s="18">
+        <v>48000</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A260" s="18">
+        <v>48030</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A261" s="18">
+        <v>48061</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A262" s="18">
+        <v>48092</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A263" s="18">
+        <v>48122</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A264" s="18">
+        <v>48153</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A265" s="18">
+        <v>48183</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A266" s="18">
+        <v>48214</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A267" s="18">
+        <v>48245</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A268" s="18">
+        <v>48274</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A269" s="18">
+        <v>48305</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A270" s="18">
+        <v>48335</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A271" s="18">
+        <v>48366</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A272" s="18">
+        <v>48396</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A273" s="18">
+        <v>48427</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A274" s="18">
+        <v>48458</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A275" s="18">
+        <v>48488</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A276" s="18">
+        <v>48519</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A277" s="18">
+        <v>48549</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A278" s="18">
+        <v>48580</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A279" s="18">
+        <v>48611</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A280" s="18">
+        <v>48639</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A281" s="18">
+        <v>48670</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A282" s="18">
+        <v>48700</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A283" s="18">
+        <v>48731</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A284" s="18">
+        <v>48761</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A285" s="18">
+        <v>48792</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A286" s="18">
+        <v>48823</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A287" s="18">
+        <v>48853</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A288" s="18">
+        <v>48884</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A289" s="18">
+        <v>48914</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A290" s="18">
+        <v>48945</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A291" s="18">
+        <v>48976</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A292" s="18">
+        <v>49004</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A293" s="18">
+        <v>49035</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A294" s="18">
+        <v>49065</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A295" s="18">
+        <v>49096</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A296" s="18">
+        <v>49126</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A297" s="18">
+        <v>49157</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A298" s="18">
+        <v>49188</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A299" s="18">
+        <v>49218</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A300" s="18">
+        <v>49249</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A301" s="18">
+        <v>49279</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A302" s="18">
+        <v>49310</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A303" s="18">
+        <v>49341</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A304" s="18">
+        <v>49369</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A305" s="18">
+        <v>49400</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A306" s="18">
+        <v>49430</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A307" s="18">
+        <v>49461</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A308" s="18">
+        <v>49491</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A309" s="18">
+        <v>49522</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A310" s="18">
+        <v>49553</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A311" s="18">
+        <v>49583</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A312" s="18">
+        <v>49614</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A313" s="18">
+        <v>49644</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A314" s="18">
+        <v>49675</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A315" s="18">
+        <v>49706</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A316" s="18">
+        <v>49735</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A317" s="18">
+        <v>49766</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A318" s="18">
+        <v>49796</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A319" s="18">
+        <v>49827</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A320" s="18">
+        <v>49857</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A321" s="18">
+        <v>49888</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A322" s="18">
+        <v>49919</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A323" s="18">
+        <v>49949</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A324" s="18">
+        <v>49980</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A325" s="18">
+        <v>50010</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A326" s="18">
+        <v>50041</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A327" s="18">
+        <v>50072</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A328" s="18">
+        <v>50100</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A329" s="18">
+        <v>50131</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A330" s="18">
+        <v>50161</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A331" s="18">
+        <v>50192</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A332" s="18">
+        <v>50222</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A333" s="18">
+        <v>50253</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A334" s="18">
+        <v>50284</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A335" s="18">
+        <v>50314</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A336" s="18">
+        <v>50345</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A337" s="18">
+        <v>50375</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A338" s="18">
+        <v>50406</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A339" s="18">
+        <v>50437</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A340" s="18">
+        <v>50465</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A341" s="18">
+        <v>50496</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A342" s="18">
+        <v>50526</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A343" s="18">
+        <v>50557</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A344" s="18">
+        <v>50587</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A345" s="18">
+        <v>50618</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A346" s="18">
+        <v>50649</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A347" s="18">
+        <v>50679</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A348" s="18">
+        <v>50710</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A349" s="18">
+        <v>50740</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A350" s="18">
+        <v>50771</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A351" s="18">
+        <v>50802</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A352" s="18">
+        <v>50830</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A353" s="18">
+        <v>50861</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A354" s="18">
+        <v>50891</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A355" s="18">
+        <v>50922</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A356" s="18">
+        <v>50952</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A357" s="18">
+        <v>50983</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A358" s="18">
+        <v>51014</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A359" s="18">
+        <v>51044</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A360" s="18">
+        <v>51075</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A361" s="18">
+        <v>51105</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A362" s="18">
+        <v>51136</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A363" s="18">
+        <v>51167</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A364" s="18">
+        <v>51196</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A365" s="18">
+        <v>51227</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A366" s="18">
+        <v>51257</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A367" s="18">
+        <v>51288</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A368" s="18">
+        <v>51318</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A369" s="18">
+        <v>51349</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A370" s="18">
+        <v>51380</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A371" s="18">
+        <v>51410</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A372" s="18">
+        <v>51441</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A373" s="18">
+        <v>51471</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A374" s="18">
+        <v>51502</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A375" s="18">
+        <v>51533</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A376" s="18">
+        <v>51561</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A377" s="18">
+        <v>51592</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A378" s="18">
+        <v>51622</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A379" s="18">
+        <v>51653</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A380" s="18">
+        <v>51683</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A381" s="18">
+        <v>51714</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A382" s="18">
+        <v>51745</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A383" s="18">
+        <v>51775</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A384" s="18">
+        <v>51806</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A385" s="18">
+        <v>51836</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A386" s="18">
+        <v>51867</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A387" s="18">
+        <v>51898</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A388" s="18">
+        <v>51926</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A389" s="18">
+        <v>51957</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A390" s="18">
+        <v>51987</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A391" s="18">
+        <v>52018</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A392" s="18">
+        <v>52048</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A393" s="18">
+        <v>52079</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A394" s="18">
+        <v>52110</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A395" s="18">
+        <v>52140</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A396" s="18">
+        <v>52171</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A397" s="18">
+        <v>52201</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A398" s="18"/>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A399" s="18"/>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A400" s="18"/>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A401" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809F9B9C-1920-5444-AB59-3DDCE6BBBC45}">
+  <sheetPr>
+    <tabColor theme="3" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:A397"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="18">
+        <v>40179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="18">
+        <v>40210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="18">
+        <v>40238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="18">
+        <v>40269</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="18">
+        <v>40299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="18">
+        <v>40330</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="18">
+        <v>40360</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="18">
+        <v>40391</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="18">
+        <v>40422</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="18">
+        <v>40452</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="18">
+        <v>40483</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="18">
+        <v>40513</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="18">
+        <v>40544</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="18">
+        <v>40575</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="18">
+        <v>40603</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="18">
+        <v>40634</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="18">
+        <v>40664</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="18">
+        <v>40695</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="18">
+        <v>40725</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="18">
+        <v>40756</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="18">
+        <v>40787</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="18">
+        <v>40817</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="18">
+        <v>40848</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="18">
+        <v>40878</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="18">
+        <v>40909</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="18">
+        <v>40940</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="18">
+        <v>40969</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="18">
+        <v>41000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="18">
+        <v>41030</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="18">
+        <v>41061</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="18">
+        <v>41091</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="18">
+        <v>41122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="18">
+        <v>41153</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="18">
+        <v>41183</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="18">
+        <v>41214</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="18">
+        <v>41244</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="18">
+        <v>41275</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="18">
+        <v>41306</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="18">
+        <v>41334</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="18">
+        <v>41365</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="18">
+        <v>41395</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="18">
+        <v>41426</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="18">
+        <v>41456</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="18">
+        <v>41487</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="18">
+        <v>41518</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="18">
+        <v>41548</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="18">
+        <v>41579</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="18">
+        <v>41609</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="18">
+        <v>41640</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="18">
+        <v>41671</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="18">
+        <v>41699</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="18">
+        <v>41730</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="18">
+        <v>41760</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="18">
+        <v>41791</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="18">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="18">
+        <v>41852</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="18">
+        <v>41883</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="18">
+        <v>41913</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="18">
+        <v>41944</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="18">
+        <v>41974</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="18">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="18">
+        <v>42036</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="18">
+        <v>42064</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="18">
+        <v>42095</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="18">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="18">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="18">
+        <v>42186</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="18">
+        <v>42217</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="18">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="18">
+        <v>42278</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="18">
+        <v>42309</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="18">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="18">
+        <v>42370</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="18">
+        <v>42401</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" s="18">
+        <v>42430</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="18">
+        <v>42461</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="18">
+        <v>42491</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="18">
+        <v>42522</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" s="18">
+        <v>42552</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="18">
+        <v>42583</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="18">
+        <v>42614</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="18">
+        <v>42644</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" s="18">
+        <v>42675</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="18">
+        <v>42705</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" s="18">
+        <v>42736</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" s="18">
+        <v>42767</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" s="18">
+        <v>42795</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="18">
+        <v>42826</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" s="18">
+        <v>42856</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" s="18">
+        <v>42887</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" s="18">
+        <v>42917</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" s="18">
+        <v>42948</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" s="18">
+        <v>42979</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" s="18">
+        <v>43009</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" s="18">
+        <v>43040</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" s="18">
+        <v>43070</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" s="18">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="18">
+        <v>43132</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" s="18">
+        <v>43160</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" s="18">
+        <v>43191</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" s="18">
+        <v>43221</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" s="18">
+        <v>43252</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" s="18">
+        <v>43282</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" s="18">
+        <v>43313</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" s="18">
+        <v>43344</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" s="18">
+        <v>43374</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" s="18">
+        <v>43405</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" s="18">
+        <v>43435</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" s="18">
+        <v>43466</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" s="18">
+        <v>43497</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" s="18">
+        <v>43525</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" s="18">
+        <v>43556</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" s="18">
+        <v>43586</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" s="18">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" s="18">
+        <v>43647</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" s="18">
+        <v>43678</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" s="18">
+        <v>43709</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" s="18">
+        <v>43739</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" s="18">
+        <v>43770</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" s="18">
+        <v>43800</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" s="18">
+        <v>43831</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123" s="18">
+        <v>43862</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124" s="18">
+        <v>43891</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125" s="18">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126" s="18">
+        <v>43952</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127" s="18">
+        <v>43983</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128" s="18">
+        <v>44013</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129" s="18">
+        <v>44044</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" s="18">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" s="18">
+        <v>44105</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" s="18">
+        <v>44136</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" s="18">
+        <v>44166</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" s="18">
+        <v>44197</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" s="18">
+        <v>44228</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" s="18">
+        <v>44256</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" s="18">
+        <v>44287</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" s="18">
+        <v>44317</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" s="18">
+        <v>44348</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" s="18">
+        <v>44378</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" s="18">
+        <v>44409</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142" s="18">
+        <v>44440</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" s="18">
+        <v>44470</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144" s="18">
+        <v>44501</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145" s="18">
+        <v>44531</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146" s="18">
+        <v>44562</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147" s="18">
+        <v>44593</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148" s="18">
+        <v>44621</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149" s="18">
+        <v>44652</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150" s="18">
+        <v>44682</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151" s="18">
+        <v>44713</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152" s="18">
+        <v>44743</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153" s="18">
+        <v>44774</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154" s="18">
+        <v>44805</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155" s="18">
+        <v>44835</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156" s="18">
+        <v>44866</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" s="18">
+        <v>44896</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158" s="18">
+        <v>44927</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159" s="18">
+        <v>44958</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160" s="18">
+        <v>44986</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" s="18">
+        <v>45017</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" s="18">
+        <v>45047</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" s="18">
+        <v>45078</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" s="18">
+        <v>45108</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165" s="18">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" s="18">
+        <v>45170</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167" s="18">
+        <v>45200</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168" s="18">
+        <v>45231</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169" s="18">
+        <v>45261</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170" s="18">
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171" s="18">
+        <v>45323</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172" s="18">
+        <v>45352</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173" s="18">
+        <v>45383</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174" s="18">
+        <v>45413</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175" s="18">
+        <v>45444</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176" s="18">
+        <v>45474</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177" s="18">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" s="18">
+        <v>45536</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179" s="18">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180" s="18">
+        <v>45597</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181" s="18">
+        <v>45627</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182" s="18">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183" s="18">
+        <v>45689</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184" s="18">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185" s="18">
+        <v>45748</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186" s="18">
+        <v>45778</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187" s="18">
+        <v>45809</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188" s="18">
+        <v>45839</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189" s="18">
+        <v>45870</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190" s="18">
+        <v>45901</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191" s="18">
+        <v>45931</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192" s="18">
+        <v>45962</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193" s="18">
+        <v>45992</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A194" s="18">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195" s="18">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A196" s="18">
+        <v>46082</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A197" s="18">
+        <v>46113</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A198" s="18">
+        <v>46143</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A199" s="18">
+        <v>46174</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A200" s="18">
+        <v>46204</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201" s="18">
+        <v>46235</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A202" s="18">
+        <v>46266</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203" s="18">
+        <v>46296</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A204" s="18">
+        <v>46327</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A205" s="18">
+        <v>46357</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A206" s="18">
+        <v>46388</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A207" s="18">
+        <v>46419</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A208" s="18">
+        <v>46447</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209" s="18">
+        <v>46478</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210" s="18">
+        <v>46508</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A211" s="18">
+        <v>46539</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A212" s="18">
+        <v>46569</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213" s="18">
+        <v>46600</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A214" s="18">
+        <v>46631</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A215" s="18">
+        <v>46661</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A216" s="18">
+        <v>46692</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A217" s="18">
+        <v>46722</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A218" s="18">
+        <v>46753</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A219" s="18">
+        <v>46784</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A220" s="18">
+        <v>46813</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A221" s="18">
+        <v>46844</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A222" s="18">
+        <v>46874</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A223" s="18">
+        <v>46905</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A224" s="18">
+        <v>46935</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A225" s="18">
+        <v>46966</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A226" s="18">
+        <v>46997</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A227" s="18">
+        <v>47027</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A228" s="18">
+        <v>47058</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A229" s="18">
+        <v>47088</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A230" s="18">
+        <v>47119</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A231" s="18">
+        <v>47150</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A232" s="18">
+        <v>47178</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A233" s="18">
+        <v>47209</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A234" s="18">
+        <v>47239</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A235" s="18">
+        <v>47270</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A236" s="18">
+        <v>47300</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A237" s="18">
+        <v>47331</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A238" s="18">
+        <v>47362</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A239" s="18">
+        <v>47392</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A240" s="18">
+        <v>47423</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A241" s="18">
+        <v>47453</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A242" s="18">
+        <v>47484</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A243" s="18">
+        <v>47515</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A244" s="18">
+        <v>47543</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A245" s="18">
+        <v>47574</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A246" s="18">
+        <v>47604</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A247" s="18">
+        <v>47635</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A248" s="18">
+        <v>47665</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A249" s="18">
+        <v>47696</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A250" s="18">
+        <v>47727</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A251" s="18">
+        <v>47757</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A252" s="18">
+        <v>47788</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A253" s="18">
+        <v>47818</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A254" s="18">
+        <v>47849</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A255" s="18">
+        <v>47880</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A256" s="18">
+        <v>47908</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A257" s="18">
+        <v>47939</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A258" s="18">
+        <v>47969</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A259" s="18">
+        <v>48000</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A260" s="18">
+        <v>48030</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A261" s="18">
+        <v>48061</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A262" s="18">
+        <v>48092</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A263" s="18">
+        <v>48122</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A264" s="18">
+        <v>48153</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A265" s="18">
+        <v>48183</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A266" s="18">
+        <v>48214</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A267" s="18">
+        <v>48245</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A268" s="18">
+        <v>48274</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A269" s="18">
+        <v>48305</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A270" s="18">
+        <v>48335</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A271" s="18">
+        <v>48366</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A272" s="18">
+        <v>48396</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A273" s="18">
+        <v>48427</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A274" s="18">
+        <v>48458</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A275" s="18">
+        <v>48488</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A276" s="18">
+        <v>48519</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A277" s="18">
+        <v>48549</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A278" s="18">
+        <v>48580</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A279" s="18">
+        <v>48611</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A280" s="18">
+        <v>48639</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A281" s="18">
+        <v>48670</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A282" s="18">
+        <v>48700</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A283" s="18">
+        <v>48731</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A284" s="18">
+        <v>48761</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A285" s="18">
+        <v>48792</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A286" s="18">
+        <v>48823</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A287" s="18">
+        <v>48853</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A288" s="18">
+        <v>48884</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A289" s="18">
+        <v>48914</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A290" s="18">
+        <v>48945</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A291" s="18">
+        <v>48976</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A292" s="18">
+        <v>49004</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A293" s="18">
+        <v>49035</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A294" s="18">
+        <v>49065</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A295" s="18">
+        <v>49096</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A296" s="18">
+        <v>49126</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A297" s="18">
+        <v>49157</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A298" s="18">
+        <v>49188</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A299" s="18">
+        <v>49218</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A300" s="18">
+        <v>49249</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A301" s="18">
+        <v>49279</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A302" s="18">
+        <v>49310</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A303" s="18">
+        <v>49341</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A304" s="18">
+        <v>49369</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A305" s="18">
+        <v>49400</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A306" s="18">
+        <v>49430</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A307" s="18">
+        <v>49461</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A308" s="18">
+        <v>49491</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A309" s="18">
+        <v>49522</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A310" s="18">
+        <v>49553</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A311" s="18">
+        <v>49583</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A312" s="18">
+        <v>49614</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A313" s="18">
+        <v>49644</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A314" s="18">
+        <v>49675</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A315" s="18">
+        <v>49706</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A316" s="18">
+        <v>49735</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A317" s="18">
+        <v>49766</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A318" s="18">
+        <v>49796</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A319" s="18">
+        <v>49827</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A320" s="18">
+        <v>49857</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A321" s="18">
+        <v>49888</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A322" s="18">
+        <v>49919</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A323" s="18">
+        <v>49949</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A324" s="18">
+        <v>49980</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A325" s="18">
+        <v>50010</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A326" s="18">
+        <v>50041</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A327" s="18">
+        <v>50072</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A328" s="18">
+        <v>50100</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A329" s="18">
+        <v>50131</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A330" s="18">
+        <v>50161</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A331" s="18">
+        <v>50192</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A332" s="18">
+        <v>50222</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A333" s="18">
+        <v>50253</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A334" s="18">
+        <v>50284</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A335" s="18">
+        <v>50314</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A336" s="18">
+        <v>50345</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A337" s="18">
+        <v>50375</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A338" s="18">
+        <v>50406</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A339" s="18">
+        <v>50437</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A340" s="18">
+        <v>50465</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A341" s="18">
+        <v>50496</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A342" s="18">
+        <v>50526</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A343" s="18">
+        <v>50557</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A344" s="18">
+        <v>50587</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A345" s="18">
+        <v>50618</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A346" s="18">
+        <v>50649</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A347" s="18">
+        <v>50679</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A348" s="18">
+        <v>50710</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A349" s="18">
+        <v>50740</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A350" s="18">
+        <v>50771</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A351" s="18">
+        <v>50802</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A352" s="18">
+        <v>50830</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A353" s="18">
+        <v>50861</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A354" s="18">
+        <v>50891</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A355" s="18">
+        <v>50922</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A356" s="18">
+        <v>50952</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A357" s="18">
+        <v>50983</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A358" s="18">
+        <v>51014</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A359" s="18">
+        <v>51044</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A360" s="18">
+        <v>51075</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A361" s="18">
+        <v>51105</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A362" s="18">
+        <v>51136</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A363" s="18">
+        <v>51167</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A364" s="18">
+        <v>51196</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A365" s="18">
+        <v>51227</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A366" s="18">
+        <v>51257</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A367" s="18">
+        <v>51288</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A368" s="18">
+        <v>51318</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A369" s="18">
+        <v>51349</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A370" s="18">
+        <v>51380</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A371" s="18">
+        <v>51410</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A372" s="18">
+        <v>51441</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A373" s="18">
+        <v>51471</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A374" s="18">
+        <v>51502</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A375" s="18">
+        <v>51533</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A376" s="18">
+        <v>51561</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A377" s="18">
+        <v>51592</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A378" s="18">
+        <v>51622</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A379" s="18">
+        <v>51653</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A380" s="18">
+        <v>51683</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A381" s="18">
+        <v>51714</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A382" s="18">
+        <v>51745</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A383" s="18">
+        <v>51775</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A384" s="18">
+        <v>51806</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A385" s="18">
+        <v>51836</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A386" s="18">
+        <v>51867</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A387" s="18">
+        <v>51898</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A388" s="18">
+        <v>51926</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A389" s="18">
+        <v>51957</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A390" s="18">
+        <v>51987</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A391" s="18">
+        <v>52018</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A392" s="18">
+        <v>52048</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A393" s="18">
+        <v>52079</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A394" s="18">
+        <v>52110</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A395" s="18">
+        <v>52140</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A396" s="18">
+        <v>52171</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A397" s="18">
+        <v>52201</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B135DB0-AD3F-4044-B1FF-A0D4EB51BA31}">
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:E80"/>
@@ -2277,11 +6305,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BAF0991-2698-BC44-8533-D730AF03BB1B}">
-  <sheetPr codeName="Hoja6"/>
+  <sheetPr codeName="Hoja6">
+    <tabColor theme="4" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection sqref="A1:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2504,11 +6534,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9908EB-6C2B-7640-BCA5-4F158164632C}">
-  <sheetPr codeName="Hoja7"/>
+  <sheetPr codeName="Hoja7">
+    <tabColor theme="4" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection sqref="A1:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2731,7 +6763,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6EE77F-9491-46BE-87E7-0E2AB2968C8E}">
-  <sheetPr codeName="Hoja2"/>
+  <sheetPr codeName="Hoja2">
+    <tabColor theme="6" tint="0.79998168889431442"/>
+  </sheetPr>
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView zoomScale="132" zoomScaleNormal="85" workbookViewId="0">
@@ -3222,11 +7256,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A5BF66-2E00-8740-8200-DD18588C6A6C}">
-  <sheetPr codeName="Hoja1"/>
+  <sheetPr codeName="Hoja1">
+    <tabColor theme="6" tint="0.79998168889431442"/>
+  </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3370,11 +7406,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{123C0C09-E83A-4BC0-BA11-233DE6D57A3F}">
-  <sheetPr codeName="Hoja3"/>
+  <sheetPr codeName="Hoja3">
+    <tabColor theme="6" tint="0.79998168889431442"/>
+  </sheetPr>
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4174,7 +8212,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{923386D2-4D6E-604A-B132-ECEA16641628}">
-  <sheetPr codeName="Hoja8"/>
+  <sheetPr codeName="Hoja8">
+    <tabColor theme="9" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:T1207"/>
   <sheetViews>
     <sheetView zoomScaleNormal="70" workbookViewId="0">
@@ -73602,6 +77642,9 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F76DAC9A-080C-E743-97D2-1260889B3A0A}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -73658,10 +77701,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C043D9DB-333F-264E-B19B-27C2F7211572}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -73713,33 +77759,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<Application xmlns="http://www.sap.com/cof/excel/application">
-  <Version>2</Version>
-  <Revision>2.3.1.59180</Revision>
-</Application>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e625656c-bba3-4077-8eff-14104607af5a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="92acd330-8342-45fc-be4b-65850f6282f9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003CF4D88A847C084DB84844F39084E439" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="451e82d02e108cc447a9cc14d7f86033">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="92acd330-8342-45fc-be4b-65850f6282f9" xmlns:ns3="e625656c-bba3-4077-8eff-14104607af5a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2eae878ca301ee5618ce7adadc34258d" ns2:_="" ns3:_="">
     <xsd:import namespace="92acd330-8342-45fc-be4b-65850f6282f9"/>
@@ -73940,23 +77959,53 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e625656c-bba3-4077-8eff-14104607af5a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="92acd330-8342-45fc-be4b-65850f6282f9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<Application xmlns="http://www.sap.com/cof/excel/application">
+  <Version>2</Version>
+  <Revision>2.3.1.59180</Revision>
+</Application>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62D4AD73-2F3B-41AE-8958-0F3FAF115B0E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="92acd330-8342-45fc-be4b-65850f6282f9"/>
+    <ds:schemaRef ds:uri="e625656c-bba3-4077-8eff-14104607af5a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -73976,21 +78025,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62D4AD73-2F3B-41AE-8958-0F3FAF115B0E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="92acd330-8342-45fc-be4b-65850f6282f9"/>
-    <ds:schemaRef ds:uri="e625656c-bba3-4077-8eff-14104607af5a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat: Agregar tabla por defecto en hoja Indexaciones
</commit_message>
<xml_diff>
--- a/data/segmentacion_soat.xlsx
+++ b/data/segmentacion_soat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/app-analisis-siniestralidad/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD5429F-D1BF-6344-AE4C-778084F14A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7FAA39-C50A-C042-8978-1B2D61EEDF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12460" firstSheet="3" activeTab="6" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Aperturas_Siniestros" sheetId="13" r:id="rId1"/>
@@ -1271,8 +1271,8 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1656,7 +1656,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F14" xr:uid="{22BE6280-917F-9E46-82F3-4F72A7A28E95}">
       <formula1>"Mensual,Trimestral,Semestral,Anual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H14" xr:uid="{2D0B2328-71FF-6049-A90A-0238BE6778DC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G14" xr:uid="{2D0B2328-71FF-6049-A90A-0238BE6778DC}">
       <formula1>"Ninguna,Por fecha de ocurrencia,Por fecha de movimiento"</formula1>
     </dataValidation>
   </dataValidations>
@@ -11156,7 +11156,7 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -18050,33 +18050,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e625656c-bba3-4077-8eff-14104607af5a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="92acd330-8342-45fc-be4b-65850f6282f9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<Application xmlns="http://www.sap.com/cof/excel/application">
-  <Version>2</Version>
-  <Revision>2.3.1.59180</Revision>
-</Application>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003CF4D88A847C084DB84844F39084E439" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="451e82d02e108cc447a9cc14d7f86033">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="92acd330-8342-45fc-be4b-65850f6282f9" xmlns:ns3="e625656c-bba3-4077-8eff-14104607af5a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2eae878ca301ee5618ce7adadc34258d" ns2:_="" ns3:_="">
     <xsd:import namespace="92acd330-8342-45fc-be4b-65850f6282f9"/>
@@ -18277,7 +18250,53 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e625656c-bba3-4077-8eff-14104607af5a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="92acd330-8342-45fc-be4b-65850f6282f9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<Application xmlns="http://www.sap.com/cof/excel/application">
+  <Version>2</Version>
+  <Revision>2.3.1.59180</Revision>
+</Application>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62D4AD73-2F3B-41AE-8958-0F3FAF115B0E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="92acd330-8342-45fc-be4b-65850f6282f9"/>
+    <ds:schemaRef ds:uri="e625656c-bba3-4077-8eff-14104607af5a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -18297,7 +18316,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -18305,29 +18324,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62D4AD73-2F3B-41AE-8958-0F3FAF115B0E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="92acd330-8342-45fc-be4b-65850f6282f9"/>
-    <ds:schemaRef ds:uri="e625656c-bba3-4077-8eff-14104607af5a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>